<commit_message>
Major changes. Saved intermediate results
</commit_message>
<xml_diff>
--- a/Error_mitigation/Results.xlsx
+++ b/Error_mitigation/Results.xlsx
@@ -4878,2200 +4878,2200 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>0.23693751168730642</t>
+          <t>0.4028461829922527</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>0.21669756925958134</t>
+          <t>0.3934001170632403</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>0.23693751168730642</t>
+          <t>0.522466851131679</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>0.16279529029673115</t>
+          <t>0.522466851131679</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0.3598761162607459</t>
+          <t>0.39470411483052736</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.39117238883437544</t>
+          <t>0.3510416605017608</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.3598761162607459</t>
+          <t>0.3781297692378069</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.478052529939657</t>
+          <t>0.3781297692378069</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0.6132113415271759</t>
+          <t>0.3442759087396935</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.6099255635283704</t>
+          <t>0.339952047892451</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.6132113415271759</t>
+          <t>0.2842549808452984</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.6173263137337106</t>
+          <t>0.2842549808452984</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0.4906023028578461</t>
+          <t>0.4223157629575882</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.4847242675592243</t>
+          <t>0.44173874116832285</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.4906023028578461</t>
+          <t>0.4604850760670477</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.6386749394221056</t>
+          <t>0.4604850760670477</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0.41259092615721543</t>
+          <t>0.3075003513641269</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.41218292205179724</t>
+          <t>0.31085028579104385</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.41259092615721543</t>
+          <t>0.38955394643310115</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.42686722967578355</t>
+          <t>0.38955394643310115</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0.5257747302578587</t>
+          <t>0.3796471777270532</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.5179108106515247</t>
+          <t>0.37541993393456546</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.5257747302578587</t>
+          <t>0.5381622446492834</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.5689954538071471</t>
+          <t>0.5381622446492834</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0.278830522435086</t>
+          <t>0.6340683246916218</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.2792690209403284</t>
+          <t>0.5913940270401491</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.278830522435086</t>
+          <t>0.8543160381995724</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.34100141447608995</t>
+          <t>0.8543160381995724</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0.7311391128909118</t>
+          <t>0.47354762445623655</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.6162305940013473</t>
+          <t>0.47197126322065514</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.7311391128909118</t>
+          <t>0.5276744951717454</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.9821136729513481</t>
+          <t>0.5276744951717454</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0.5812568348298194</t>
+          <t>0.5572413867872954</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.4542743828825027</t>
+          <t>0.5315762005201982</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.5812568348298194</t>
+          <t>0.5972331558598765</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.692861274058597</t>
+          <t>0.5972331558598765</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0.40770094499229526</t>
+          <t>0.6515003225850866</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.4164831113822224</t>
+          <t>0.6516119963947736</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.40770094499229526</t>
+          <t>0.7142826577945499</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.4598142783789699</t>
+          <t>0.7142826577945499</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0.19590361762813546</t>
+          <t>0.27774467577553047</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.20537385548843473</t>
+          <t>0.26495436340909206</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.19590361762813546</t>
+          <t>0.314299985972592</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.32564433679147176</t>
+          <t>0.314299985972592</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0.324048445050449</t>
+          <t>0.46898194915145763</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.21227694146889492</t>
+          <t>0.42853793903171195</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.324048445050449</t>
+          <t>0.6135587671083143</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.8014929088341887</t>
+          <t>0.6135587671083143</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0.42753364047832554</t>
+          <t>0.44306570497679154</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.42784561202341803</t>
+          <t>0.4702106265804134</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.42753364047832554</t>
+          <t>0.49138561647589013</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.4015452443818029</t>
+          <t>0.49138561647589013</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0.7125785556237204</t>
+          <t>0.512956518198249</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.6764114385311519</t>
+          <t>0.4516976170726567</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.7125785556237204</t>
+          <t>0.8455407534021695</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.9752191762064802</t>
+          <t>0.8455407534021695</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>0.38765916289692914</t>
+          <t>0.5130617222678133</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.38117405896062295</t>
+          <t>0.4581989877733015</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.38765916289692914</t>
+          <t>0.8228809287554566</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.3737006852095326</t>
+          <t>0.8228809287554566</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0.6660308947316614</t>
+          <t>0.4699835311224983</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0.5350830581933427</t>
+          <t>0.4695367662916179</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.6660308947316614</t>
+          <t>0.5536094141587566</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.8890498075525524</t>
+          <t>0.5536094141587566</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0.5637359563716091</t>
+          <t>0.39343338825007373</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0.5294810155099137</t>
+          <t>0.29602779918313277</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.5637359563716091</t>
+          <t>0.6232818648168673</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.6415373121279905</t>
+          <t>0.6232818648168673</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0.6015735596088582</t>
+          <t>0.3115181244400112</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.5535038150869159</t>
+          <t>0.30171583021918147</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.6015735596088582</t>
+          <t>0.2666303163273112</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.6897264250990778</t>
+          <t>0.2666303163273112</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0.29324120566582806</t>
+          <t>0.5378581145040757</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0.34453098779716446</t>
+          <t>0.5180560502877868</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.29324120566582806</t>
+          <t>0.5827592889141098</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.4163891000776607</t>
+          <t>0.5827592889141098</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>0.48226569766983224</t>
+          <t>0.5525426865067933</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0.5189695352253942</t>
+          <t>0.5593949858143006</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.48226569766983224</t>
+          <t>0.512060528944456</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.8558984296920752</t>
+          <t>0.512060528944456</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>0.6693944837889982</t>
+          <t>0.6657182816506734</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0.5967518474202964</t>
+          <t>0.6398911198288844</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.6693944837889982</t>
+          <t>0.7396939896616579</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.7798733257321193</t>
+          <t>0.7396939896616579</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>0.20082780035617087</t>
+          <t>0.2403087888340336</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0.19067891594944134</t>
+          <t>0.25072670408669606</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.20082780035617087</t>
+          <t>0.34215895826869763</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.2771789599007225</t>
+          <t>0.34215895826869763</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>0.21667277983873806</t>
+          <t>0.5771017947181242</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0.21709578377252373</t>
+          <t>0.5648692213545272</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.21667277983873806</t>
+          <t>0.6555430180286396</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.24222200477499345</t>
+          <t>0.6555430180286396</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>0.15967026543954407</t>
+          <t>0.4736962392203148</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0.1460457771685209</t>
+          <t>0.4602674337619381</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.15967026543954407</t>
+          <t>0.5912917054375262</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.3631979438388309</t>
+          <t>0.5912917054375262</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>0.827538969033788</t>
+          <t>0.25050218027247695</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0.8264189840258305</t>
+          <t>0.19821605960548153</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.827538969033788</t>
+          <t>0.3106507883854148</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.850752489833311</t>
+          <t>0.3106507883854148</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>0.397305835221235</t>
+          <t>0.4171644483331785</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>0.3887230267634105</t>
+          <t>0.40450526081853605</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.397305835221235</t>
+          <t>0.626284650539274</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.648025549958496</t>
+          <t>0.626284650539274</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>0.1942784862673719</t>
+          <t>0.603644825108261</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>0.1969769795412035</t>
+          <t>0.5839123680500172</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.1942784862673719</t>
+          <t>0.8845127182795597</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.262548322366992</t>
+          <t>0.8845127182795597</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>0.2435229858166465</t>
+          <t>0.42001603424176587</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0.27363662986459336</t>
+          <t>0.37470412878883275</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.2435229858166465</t>
+          <t>0.6828897467319219</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.5509585546719918</t>
+          <t>0.6828897467319219</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>0.7184857600271986</t>
+          <t>0.621210954498089</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0.7037886823641946</t>
+          <t>0.5816196364545928</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.7184857600271986</t>
+          <t>0.882526456777025</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.7589041532428414</t>
+          <t>0.882526456777025</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>0.27369454644883134</t>
+          <t>0.7003191407836713</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0.30473112889997317</t>
+          <t>0.6993421663047688</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.27369454644883134</t>
+          <t>0.7284511305977882</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.5853295403755182</t>
+          <t>0.7284511305977882</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>0.445362900553983</t>
+          <t>0.23823942564684136</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>0.31545527800711237</t>
+          <t>0.25680446925823386</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.445362900553983</t>
+          <t>0.4629914982363573</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.5856991918254775</t>
+          <t>0.4629914982363573</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>0.509981916698717</t>
+          <t>0.33563289420073444</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>0.5030653496436305</t>
+          <t>0.32403400809215194</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.509981916698717</t>
+          <t>0.3208671892884648</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.5920347920757394</t>
+          <t>0.3208671892884648</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>0.28626071001629316</t>
+          <t>0.5896107608658752</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>0.31364592765024807</t>
+          <t>0.6188317125507431</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.28626071001629316</t>
+          <t>0.7309863629151742</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.3729352633182643</t>
+          <t>0.7309863629151742</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>0.814401750227659</t>
+          <t>0.45269495746079974</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>0.7512724094640096</t>
+          <t>0.46948097478485035</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.814401750227659</t>
+          <t>0.5347421027967143</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.9607341112033423</t>
+          <t>0.5347421027967143</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>0.4816681982365437</t>
+          <t>0.37141332168009505</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>0.47848253417889397</t>
+          <t>0.3756239951812243</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.4816681982365437</t>
+          <t>0.37332915229919633</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.5030223490779236</t>
+          <t>0.37332915229919633</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>0.3626736443668397</t>
+          <t>0.24052778169908817</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0.3408037044697914</t>
+          <t>0.28599798034653323</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.3626736443668397</t>
+          <t>0.6483952428321076</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.49194394007764686</t>
+          <t>0.6483952428321076</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>0.4583761728032195</t>
+          <t>0.2977130485903888</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>0.4636591418407989</t>
+          <t>0.2870209255063311</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.4583761728032195</t>
+          <t>0.3386897745770096</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.8106152459326937</t>
+          <t>0.3386897745770096</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>0.34116531446835174</t>
+          <t>0.4550346791711739</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>0.2983500351858664</t>
+          <t>0.4569113476697596</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>0.34116531446835174</t>
+          <t>0.5382917358387007</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.43715332220220665</t>
+          <t>0.5382917358387007</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>0.5971980468925763</t>
+          <t>0.30677801414130373</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>0.6080297199935053</t>
+          <t>0.3080532081059337</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>0.5971980468925763</t>
+          <t>0.41098111601344384</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.6269101083637435</t>
+          <t>0.41098111601344384</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>0.2799496056059013</t>
+          <t>0.24631411151150218</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>0.2820864174903344</t>
+          <t>0.26059929065604714</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.2799496056059013</t>
+          <t>0.5254730449851787</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.2694988614019482</t>
+          <t>0.5254730449851787</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>0.43599380326149606</t>
+          <t>0.47316979422804106</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>0.40546124287540103</t>
+          <t>0.5067348526492346</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>0.43599380326149606</t>
+          <t>0.6889696169227348</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0.5352018752150502</t>
+          <t>0.6889696169227348</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>0.43514597596462223</t>
+          <t>0.7407962833842455</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>0.39302932490957665</t>
+          <t>0.7418244108340897</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>0.43514597596462223</t>
+          <t>0.7448560246502302</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.5186789346190375</t>
+          <t>0.7448560246502302</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>0.26616448396647246</t>
+          <t>0.5263005999778552</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0.26091014722340783</t>
+          <t>0.4173174236267669</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0.26616448396647246</t>
+          <t>0.672731190035358</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.34620809434959715</t>
+          <t>0.672731190035358</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>0.45798732102428347</t>
+          <t>0.6126407267371008</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>0.4527447450795416</t>
+          <t>0.5234122595916276</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.45798732102428347</t>
+          <t>0.7287341551123612</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.6301041186936374</t>
+          <t>0.7287341551123612</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>0.6772306425952099</t>
+          <t>0.44956825643404663</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>0.6609685535927344</t>
+          <t>0.42561771424902894</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.6772306425952099</t>
+          <t>0.5472117945241974</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.7166777695404548</t>
+          <t>0.5472117945241974</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>0.62079201187027</t>
+          <t>0.5251172823418162</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>0.6224440779439474</t>
+          <t>0.5480278642013295</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.62079201187027</t>
+          <t>0.4975910535474399</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.8361428033996399</t>
+          <t>0.4975910535474399</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>0.439063739204362</t>
+          <t>0.7360536609669002</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>0.4377452651636988</t>
+          <t>0.7303152611006534</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.439063739204362</t>
+          <t>0.7359828773239204</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.476673652366148</t>
+          <t>0.7359828773239204</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>0.31894429411796127</t>
+          <t>0.2733109270724626</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>0.3119329566886561</t>
+          <t>0.324532516112594</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.31894429411796127</t>
+          <t>0.4124955741847445</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.2964068197406061</t>
+          <t>0.4124955741847445</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>0.3236915647897752</t>
+          <t>0.42133730955408305</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>0.35692230260614294</t>
+          <t>0.38494085903913366</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.3236915647897752</t>
+          <t>0.7858797185256425</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.6003069181587432</t>
+          <t>0.7858797185256425</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>0.21774573415397486</t>
+          <t>0.48147273621918035</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>0.3879983388663003</t>
+          <t>0.4471828626049073</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>0.21774573415397486</t>
+          <t>0.6140201490496904</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.5098254888917304</t>
+          <t>0.6140201490496904</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>0.42423546431886056</t>
+          <t>0.3272151751511388</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>0.4264738252465548</t>
+          <t>0.3353366632033717</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>0.42423546431886056</t>
+          <t>0.40170340628927403</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0.4943571046564129</t>
+          <t>0.40170340628927403</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>0.5601474801944568</t>
+          <t>0.34379016352083264</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>0.5490921839358086</t>
+          <t>0.3519881248151732</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0.5601474801944568</t>
+          <t>0.43682011145350486</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.6847974107456907</t>
+          <t>0.43682011145350486</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>0.5619106869262915</t>
+          <t>0.41240689480844006</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>0.5527363708166934</t>
+          <t>0.22498549303210555</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.5619106869262915</t>
+          <t>0.47130258208391</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.6477809732874111</t>
+          <t>0.47130258208391</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>0.6811866911684854</t>
+          <t>0.46058861769168363</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>0.6326648024954854</t>
+          <t>0.4864740767997602</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>0.6811866911684854</t>
+          <t>0.7659898123295706</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.7556903989406096</t>
+          <t>0.7659898123295706</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>0.2548614720634443</t>
+          <t>0.5278829930625187</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>0.27443268078437033</t>
+          <t>0.5362715412948664</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>0.2548614720634443</t>
+          <t>0.5737747590800809</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.17164971226088108</t>
+          <t>0.5737747590800809</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>0.2931962062781059</t>
+          <t>0.3109699337266493</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>0.30386377181900154</t>
+          <t>0.3189972779467653</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.2931962062781059</t>
+          <t>0.21434762968882207</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.43357219393927</t>
+          <t>0.21434762968882207</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>0.4320824323993405</t>
+          <t>0.6162254504759301</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>0.42114446443941217</t>
+          <t>0.6088716224189161</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.4320824323993405</t>
+          <t>0.6608258909571587</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.40571321008955696</t>
+          <t>0.6608258909571587</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>0.9564875887037547</t>
+          <t>0.28239979672332755</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>0.9557296554455293</t>
+          <t>0.25403348180118307</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0.9564875887037547</t>
+          <t>0.4430007991823949</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.9593159290976366</t>
+          <t>0.4430007991823949</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>0.3478666128149321</t>
+          <t>0.47992075618651503</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>0.3198588717296979</t>
+          <t>0.47796983607936094</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.3478666128149321</t>
+          <t>0.4723713355024761</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.779447061715284</t>
+          <t>0.4723713355024761</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>0.40127139151140984</t>
+          <t>0.8781137904713341</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>0.38771422640535447</t>
+          <t>0.8557643646617263</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0.40127139151140984</t>
+          <t>0.9459856843009904</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.49930716177907125</t>
+          <t>0.9459856843009904</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>0.31139306047329024</t>
+          <t>0.2991049264529598</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>0.30354144306211445</t>
+          <t>0.32750648993540454</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.31139306047329024</t>
+          <t>0.7112342174023768</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.35579260927680206</t>
+          <t>0.7112342174023768</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>0.4621593991045514</t>
+          <t>0.6037477312455303</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>0.4734758990920175</t>
+          <t>0.6087529988511492</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>0.4621593991045514</t>
+          <t>0.8836834958793022</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.5165480714523418</t>
+          <t>0.8836834958793022</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>0.2976161893880674</t>
+          <t>0.14203266268442888</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>0.2665539590478978</t>
+          <t>0.25271827943312297</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>0.2976161893880674</t>
+          <t>0.4364255125016505</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.6743834028637664</t>
+          <t>0.4364255125016505</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>0.669603021481747</t>
+          <t>0.7593476532016793</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>0.6703564191026359</t>
+          <t>0.7371055169234579</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>0.669603021481747</t>
+          <t>0.9378366409730127</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.7131861672562799</t>
+          <t>0.9378366409730127</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>0.7656995652961724</t>
+          <t>0.34426020210877445</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>0.7657783926020357</t>
+          <t>0.34650666696934296</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>0.7656995652961724</t>
+          <t>0.5065253893638144</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0.7913809466490423</t>
+          <t>0.5065253893638144</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>0.5357274944547512</t>
+          <t>0.4484699824354523</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>0.5263692135533302</t>
+          <t>0.4599137513251942</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>0.5357274944547512</t>
+          <t>0.44983654547555335</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0.6042445892767968</t>
+          <t>0.44983654547555335</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>0.5171191511561655</t>
+          <t>0.4524022124607895</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>0.47153926356654907</t>
+          <t>0.4298516130312733</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>0.5171191511561655</t>
+          <t>0.5100996544383871</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>0.7913920545471674</t>
+          <t>0.5100996544383871</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>0.5415859498399325</t>
+          <t>0.4974081168520049</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>0.5799187823400205</t>
+          <t>0.5189715558615233</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>0.5415859498399325</t>
+          <t>0.6272584040276936</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0.8020731907296824</t>
+          <t>0.6272584040276936</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>0.5041233609431944</t>
+          <t>0.5599800023175177</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>0.457882995126915</t>
+          <t>0.5682599422978903</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0.5041233609431944</t>
+          <t>0.6007733441846014</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.6183180990164969</t>
+          <t>0.6007733441846014</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>0.7824946111150679</t>
+          <t>0.44829224558258146</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0.7779999437310657</t>
+          <t>0.4478852878960648</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>0.7824946111150679</t>
+          <t>0.623229217215235</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>0.8488784355442697</t>
+          <t>0.623229217215235</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>0.6338341097824477</t>
+          <t>0.6206749343570195</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>0.6589622154900225</t>
+          <t>0.5904439452898204</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0.6338341097824477</t>
+          <t>0.6879612609206869</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.8438238608588129</t>
+          <t>0.6879612609206869</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>0.5272381320670251</t>
+          <t>0.47446985887224485</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>0.5088773273100488</t>
+          <t>0.3791502282183891</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>0.5272381320670251</t>
+          <t>0.7225676183347159</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.6948604936059253</t>
+          <t>0.7225676183347159</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>0.7419693938166928</t>
+          <t>0.5294815744182304</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>0.5990558157645286</t>
+          <t>0.5173977956624799</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>0.7419693938166928</t>
+          <t>0.6153626477490391</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.9568199837104231</t>
+          <t>0.6153626477490391</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>0.6479336614270992</t>
+          <t>0.36429862336014884</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>0.5847085007961788</t>
+          <t>0.3104582584583381</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>0.6479336614270992</t>
+          <t>0.731221670508789</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.6693840454637034</t>
+          <t>0.731221670508789</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>0.6000642652452036</t>
+          <t>0.5464263223145331</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>0.515311889533115</t>
+          <t>0.539804412620533</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>0.6000642652452036</t>
+          <t>0.6676168688002324</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>0.8118281650637732</t>
+          <t>0.6676168688002324</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>0.4765473118012328</t>
+          <t>0.4183243183290414</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>0.4854800014945224</t>
+          <t>0.41074121486871135</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>0.4765473118012328</t>
+          <t>0.44668199505480655</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>0.43848918721176466</t>
+          <t>0.44668199505480655</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>0.15827257048650564</t>
+          <t>0.2959113381333811</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>0.16280381585289316</t>
+          <t>0.3000318602521064</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>0.15827257048650564</t>
+          <t>0.33526372225220136</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>0.06828488937428283</t>
+          <t>0.33526372225220136</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>0.23986515332305397</t>
+          <t>0.6390881531430556</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>0.2452786108250725</t>
+          <t>0.5872105985454217</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>0.23986515332305397</t>
+          <t>0.9042035314289257</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>0.384664119453628</t>
+          <t>0.9042035314289257</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>0.41714153046170177</t>
+          <t>0.48931930736367024</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>0.4046536266034627</t>
+          <t>0.48245125284329576</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>0.41714153046170177</t>
+          <t>0.4925046133809086</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>0.778060020916689</t>
+          <t>0.4925046133809086</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>0.34758449378900025</t>
+          <t>0.5148357075786226</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>0.34547263076463586</t>
+          <t>0.5152659845992348</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>0.34758449378900025</t>
+          <t>0.6358084031750758</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>0.41752325548201713</t>
+          <t>0.6358084031750758</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>0.6934230118128166</t>
+          <t>0.47954157773458783</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>0.6701406188463579</t>
+          <t>0.3048459735858408</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>0.6934230118128166</t>
+          <t>0.8975697213933733</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>0.7318206763118893</t>
+          <t>0.8975697213933733</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>0.5846892726735516</t>
+          <t>0.4868418823505674</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.5652604726651254</t>
+          <t>0.4683681219443869</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>0.5846892726735516</t>
+          <t>0.5060274106464507</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>0.6423521326896202</t>
+          <t>0.5060274106464507</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>0.41093610925106117</t>
+          <t>0.47904949317669265</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>0.40709263068843693</t>
+          <t>0.4306237251033198</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>0.41093610925106117</t>
+          <t>0.8186563355707295</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>0.36957703337512643</t>
+          <t>0.8186563355707295</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>0.2596642737643138</t>
+          <t>0.4254631831730261</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>0.22550719780302605</t>
+          <t>0.37159723927564076</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0.2596642737643138</t>
+          <t>0.6157470988301398</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>0.25777758655821625</t>
+          <t>0.6157470988301398</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>0.7909572773874629</t>
+          <t>0.47610331575294196</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>0.755401270206617</t>
+          <t>0.4536418757151149</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>0.7909572773874629</t>
+          <t>0.5536914506999268</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>0.9063960214915571</t>
+          <t>0.5536914506999268</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>0.44763768430540335</t>
+          <t>0.5208967091639289</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>0.3710708729808027</t>
+          <t>0.4541687816488902</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>0.44763768430540335</t>
+          <t>0.9671123257102889</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>0.8705389208234516</t>
+          <t>0.9671123257102889</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>0.44775582612233883</t>
+          <t>0.5799384877974917</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>0.33944282289654304</t>
+          <t>0.5865360489110654</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>0.44775582612233883</t>
+          <t>0.7510795753635211</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>0.7429968681048256</t>
+          <t>0.7510795753635211</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>0.7276676065810674</t>
+          <t>0.5430756082939625</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>0.7098486596313557</t>
+          <t>0.5365835576979047</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>0.7276676065810674</t>
+          <t>0.5478752038192009</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>0.6568264981800401</t>
+          <t>0.5478752038192009</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>0.41766004886872465</t>
+          <t>0.5824138052214625</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>0.41160924422637646</t>
+          <t>0.5822724712179633</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>0.41766004886872465</t>
+          <t>0.7062050907818428</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>0.46935458392097107</t>
+          <t>0.7062050907818428</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>0.5928355511016272</t>
+          <t>0.15884778510906097</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>0.5914002623038698</t>
+          <t>0.1697640104275699</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>0.5928355511016272</t>
+          <t>0.42190812114760146</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>0.48401884910657855</t>
+          <t>0.42190812114760146</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>0.47992869471786465</t>
+          <t>0.5223300493087263</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>0.47848220077768855</t>
+          <t>0.512820547692263</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>0.47992869471786465</t>
+          <t>0.6472940640796094</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>0.695045046967674</t>
+          <t>0.6472940640796094</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>0.533391122099649</t>
+          <t>0.6217589105476383</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>0.5189276063805399</t>
+          <t>0.6193692903743334</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>0.533391122099649</t>
+          <t>0.6964178980617316</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>0.5395746969887646</t>
+          <t>0.6964178980617316</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>0.2517630505587529</t>
+          <t>0.5877991369162332</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>0.25399593590979375</t>
+          <t>0.5626615756935898</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>0.2517630505587529</t>
+          <t>0.7251510442050956</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>0.49779621423600884</t>
+          <t>0.7251510442050956</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>0.1991130054571104</t>
+          <t>0.3492472031568411</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>0.1822896314794341</t>
+          <t>0.3184997177753972</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>0.1991130054571104</t>
+          <t>0.350140173545769</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>0.7299303720064205</t>
+          <t>0.350140173545769</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>0.5392471655993255</t>
+          <t>0.4125649712924288</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>0.48459672321331854</t>
+          <t>0.31112297005391487</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>0.5392471655993255</t>
+          <t>0.6116011172039196</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>0.8564047207817029</t>
+          <t>0.6116011172039196</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>0.2617829561450387</t>
+          <t>0.6234356754998857</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>0.2639109489859763</t>
+          <t>0.521808771192042</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>0.2617829561450387</t>
+          <t>0.7100920278255735</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>0.46855947880585364</t>
+          <t>0.7100920278255735</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>0.4859794890533857</t>
+          <t>0.6455452538943025</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>0.3846516118975527</t>
+          <t>0.5501520570704943</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>0.4859794890533857</t>
+          <t>0.80934962216455</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>0.6698615547097071</t>
+          <t>0.80934962216455</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>0.5108057686090348</t>
+          <t>0.5244275068157568</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>0.48633823711509333</t>
+          <t>0.32378298303674924</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>0.5108057686090348</t>
+          <t>0.6452872065558158</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>0.6301125773771662</t>
+          <t>0.6452872065558158</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>0.3907834464680905</t>
+          <t>0.3438142569415877</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>0.6080421549170376</t>
+          <t>0.3273270072462326</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>0.3907834464680905</t>
+          <t>0.4872630646603954</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>0.8653735263787854</t>
+          <t>0.4872630646603954</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>0.7735142522248978</t>
+          <t>0.7092915379639296</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>0.7090545482219407</t>
+          <t>0.6855163876580801</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>0.7735142522248978</t>
+          <t>0.738317482489388</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>0.7886333256641597</t>
+          <t>0.738317482489388</t>
         </is>
       </c>
     </row>

</xml_diff>